<commit_message>
Concertando acervo M - J. 2021
</commit_message>
<xml_diff>
--- a/Acervos Janeiro e fevereiro de 2021 - 1º Grau.xlsx
+++ b/Acervos Janeiro e fevereiro de 2021 - 1º Grau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99d2b5f2c1860f7d/Documentos/PRODUTIVIDADE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{54EF2DB4-9250-4CAF-9FC4-71B632E37C87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{55DE36C8-5A06-4DD9-8482-BDD664A404CE}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{54EF2DB4-9250-4CAF-9FC4-71B632E37C87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{AB6F48F8-0411-4AEB-ADFE-7DB79F9883D4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5418E676-3F12-4F39-86DA-3564FB697F38}"/>
   </bookViews>
@@ -1137,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F7A559-DDF2-4EF9-AF7A-D69EC408705A}">
   <dimension ref="A1:F447"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F172" sqref="F172"/>
+    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B185" sqref="B185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>